<commit_message>
completed the tests of BankAccount and filled out  the test plan table and finished the def main function as required
</commit_message>
<xml_diff>
--- a/tests/A01_pixell_test_plan_bank_account.xlsx
+++ b/tests/A01_pixell_test_plan_bank_account.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lauri\Desktop\Intermediate Software Development0315\2. Assignments\updated_again_0416\assignment_01\starter (given)\tests\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ADD\Term2\intermediate_software_development\project\Assignment_01\isd_project\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56DA4A4F-2E79-4753-B9BE-A428E4C99413}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9F9736C-F182-4C9D-AC96-903D6AAE1253}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31140" yWindow="2340" windowWidth="25185" windowHeight="13845" xr2:uid="{8D9DD509-55B1-455D-8036-16809AD15960}"/>
+    <workbookView xWindow="6210" yWindow="0" windowWidth="15788" windowHeight="12863" xr2:uid="{8D9DD509-55B1-455D-8036-16809AD15960}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -183,7 +183,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="63">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -248,9 +248,6 @@
     <t>correctly updates balance attribute when negative amount is received.</t>
   </si>
   <si>
-    <t>Balance attribute value remains unchanged when amount is non-numeric</t>
-  </si>
-  <si>
     <t>__str__</t>
   </si>
   <si>
@@ -282,6 +279,99 @@
   </si>
   <si>
     <t>returns client number attribute</t>
+  </si>
+  <si>
+    <t>account_number:123,       client_number:456,  balance:1000.00</t>
+  </si>
+  <si>
+    <t>The bank_account instance is created successfully with the attributes correctly set.</t>
+  </si>
+  <si>
+    <t>account_number:"123",       client_number:456,  balance:1000.00</t>
+  </si>
+  <si>
+    <t>successfully raise ValueError as setted</t>
+  </si>
+  <si>
+    <t>account_number:"123",       client_number:456,  balance:"balance"</t>
+  </si>
+  <si>
+    <t>the value of balance attribute is setted to 0.0 successfully</t>
+  </si>
+  <si>
+    <t>account_number:123,       client_number:"456",  balance:1000.00</t>
+  </si>
+  <si>
+    <t>Balance attribute successfully converted to a float</t>
+  </si>
+  <si>
+    <t>account_number:123,       client_number:"456",  balance:1000</t>
+  </si>
+  <si>
+    <t>the value of balance attribute is converted to a float successfully</t>
+  </si>
+  <si>
+    <t>account_number:123</t>
+  </si>
+  <si>
+    <t>successfully return account_number</t>
+  </si>
+  <si>
+    <t>successfully return client_number</t>
+  </si>
+  <si>
+    <t>client_number:456</t>
+  </si>
+  <si>
+    <t>balance:1000.00</t>
+  </si>
+  <si>
+    <t>successfully return balance</t>
+  </si>
+  <si>
+    <t>amount =200</t>
+  </si>
+  <si>
+    <t>successfully update balance and result is as expected</t>
+  </si>
+  <si>
+    <t>amount =-200</t>
+  </si>
+  <si>
+    <t>amount ="amount"</t>
+  </si>
+  <si>
+    <t>amount = 200</t>
+  </si>
+  <si>
+    <t>amount =- 200</t>
+  </si>
+  <si>
+    <t>Balance attribute value remains unchanged and raise ValueError  when amount is non-numeric</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> raise ValueError  when amount is invalid</t>
+  </si>
+  <si>
+    <t>successfully added amount to the current balance</t>
+  </si>
+  <si>
+    <t>ValueError when amount is non-numeric</t>
+  </si>
+  <si>
+    <t>ValueError when not positive amount is provided.</t>
+  </si>
+  <si>
+    <t>amount = 0</t>
+  </si>
+  <si>
+    <t>amount = 1100</t>
+  </si>
+  <si>
+    <t>successfully subtract amount from balance</t>
+  </si>
+  <si>
+    <t>successfully return a string as setted</t>
   </si>
 </sst>
 </file>
@@ -616,8 +706,11 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -643,11 +736,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -861,7 +951,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7B0B8C9F-A34D-46F3-9066-19FDAF76B033}" name="Table1" displayName="Table1" ref="B6:G37" totalsRowShown="0" headerRowDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7B0B8C9F-A34D-46F3-9066-19FDAF76B033}" name="Table1" displayName="Table1" ref="B6:G40" totalsRowShown="0" headerRowDxfId="6">
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{B4BB882C-2019-4F87-8900-426FA9A11FFB}" name="Test Case ID" dataDxfId="5"/>
     <tableColumn id="2" xr3:uid="{1904C92F-9639-4229-AA4E-4C4DEAF21EEE}" name="Method being Tested" dataDxfId="4"/>
@@ -1191,55 +1281,55 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DADEBCC4-BB44-48CD-B9AB-1E2FD3EE0EEB}">
-  <dimension ref="B1:G39"/>
+  <dimension ref="B1:G42"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7:D22"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="12.7109375" customWidth="1"/>
-    <col min="3" max="3" width="22.28515625" customWidth="1"/>
-    <col min="4" max="4" width="32.7109375" customWidth="1"/>
-    <col min="5" max="5" width="27.140625" customWidth="1"/>
-    <col min="6" max="6" width="28.28515625" customWidth="1"/>
-    <col min="7" max="7" width="26.42578125" customWidth="1"/>
+    <col min="2" max="2" width="7.265625" customWidth="1"/>
+    <col min="3" max="3" width="16.9296875" customWidth="1"/>
+    <col min="4" max="4" width="30.265625" customWidth="1"/>
+    <col min="5" max="5" width="8.19921875" customWidth="1"/>
+    <col min="6" max="6" width="18.19921875" customWidth="1"/>
+    <col min="7" max="7" width="26.3984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:7" ht="73.150000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="1.45">
+    <row r="1" spans="2:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="2" spans="2:7" ht="73.150000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="2.85">
       <c r="B2" s="2" t="e" vm="1">
         <v>#VALUE!</v>
       </c>
-      <c r="C2" s="14" t="s">
+      <c r="C2" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15"/>
-      <c r="G2" s="15"/>
-    </row>
-    <row r="3" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="16"/>
+    </row>
+    <row r="3" spans="2:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B3" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="16"/>
-      <c r="D3" s="17"/>
-    </row>
-    <row r="4" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C3" s="17"/>
+      <c r="D3" s="18"/>
+    </row>
+    <row r="4" spans="2:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B4" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="18" t="s">
+      <c r="C4" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="19"/>
-    </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="D4" s="20"/>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B5" s="1"/>
     </row>
-    <row r="6" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B6" s="8" t="s">
         <v>0</v>
       </c>
@@ -1259,21 +1349,25 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:7" ht="46.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B7" s="10">
         <v>1</v>
       </c>
-      <c r="C7" s="22" t="s">
+      <c r="C7" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="22" t="s">
+      <c r="D7" s="13" t="s">
         <v>10</v>
       </c>
       <c r="E7" s="11"/>
-      <c r="F7" s="11"/>
-      <c r="G7" s="11"/>
-    </row>
-    <row r="8" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F7" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="G7" s="11" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" ht="47.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B8" s="3">
         <v>2</v>
       </c>
@@ -1284,24 +1378,32 @@
         <v>13</v>
       </c>
       <c r="E8" s="12"/>
-      <c r="F8" s="11"/>
-      <c r="G8" s="12"/>
-    </row>
-    <row r="9" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="13">
+      <c r="F8" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="G8" s="12" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B9" s="10">
         <v>3</v>
       </c>
-      <c r="C9" s="23" t="s">
+      <c r="C9" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="D9" s="23" t="s">
-        <v>29</v>
+      <c r="D9" s="14" t="s">
+        <v>28</v>
       </c>
       <c r="E9" s="12"/>
-      <c r="F9" s="12"/>
-      <c r="G9" s="12"/>
-    </row>
-    <row r="10" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F9" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="G9" s="12" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" ht="43.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B10" s="10">
         <v>4</v>
       </c>
@@ -1309,211 +1411,287 @@
         <v>9</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E10" s="12"/>
-      <c r="F10" s="12"/>
-      <c r="G10" s="12"/>
-    </row>
-    <row r="11" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="10">
+      <c r="F10" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="G10" s="12" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" ht="52.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B11" s="3">
         <v>5</v>
       </c>
-      <c r="C11" s="23" t="s">
-        <v>14</v>
-      </c>
-      <c r="D11" s="23" t="s">
-        <v>15</v>
+      <c r="C11" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>39</v>
       </c>
       <c r="E11" s="12"/>
-      <c r="F11" s="12"/>
-      <c r="G11" s="12"/>
-    </row>
-    <row r="12" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F11" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="G11" s="12" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B12" s="10">
         <v>6</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C12" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="E12" s="12"/>
+      <c r="F12" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="G12" s="12" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B13" s="10">
+        <v>7</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="D13" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="D12" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="E12" s="12"/>
-      <c r="F12" s="12"/>
-      <c r="G12" s="12"/>
-    </row>
-    <row r="13" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="3">
-        <v>7</v>
-      </c>
-      <c r="C13" s="23" t="s">
+      <c r="E13" s="12"/>
+      <c r="F13" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="G13" s="12" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B14" s="3">
+        <v>8</v>
+      </c>
+      <c r="C14" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="D13" s="23" t="s">
+      <c r="D14" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="E13" s="12"/>
-      <c r="F13" s="12"/>
-      <c r="G13" s="12"/>
-    </row>
-    <row r="14" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="13">
-        <v>8</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E14" s="12"/>
-      <c r="F14" s="12"/>
-      <c r="G14" s="12"/>
-    </row>
-    <row r="15" spans="2:7" ht="47.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E14" s="10"/>
+      <c r="F14" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="G14" s="10" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B15" s="10">
         <v>9</v>
       </c>
-      <c r="C15" s="23" t="s">
+      <c r="C15" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="D15" s="23" t="s">
-        <v>20</v>
-      </c>
-      <c r="E15" s="12"/>
-      <c r="F15" s="12"/>
-      <c r="G15" s="12"/>
-    </row>
-    <row r="16" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D15" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="E15" s="10"/>
+      <c r="F15" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="G15" s="10" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" ht="47.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B16" s="10">
         <v>10</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="C16" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="D16" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E16" s="12"/>
-      <c r="F16" s="12"/>
-      <c r="G16" s="12"/>
-    </row>
-    <row r="17" spans="2:7" ht="51" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="10">
+      <c r="D16" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="E16" s="10"/>
+      <c r="F16" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="G16" s="10" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B17" s="3">
         <v>11</v>
       </c>
-      <c r="C17" s="23" t="s">
+      <c r="C17" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="D17" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="E17" s="10"/>
+      <c r="F17" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="G17" s="10" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B18" s="10">
+        <v>12</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="D18" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="E18" s="10"/>
+      <c r="F18" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="G18" s="10" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B19" s="10">
+        <v>13</v>
+      </c>
+      <c r="C19" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="D19" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="E19" s="10"/>
+      <c r="F19" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="G19" s="10" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" ht="51" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B20" s="3">
+        <v>14</v>
+      </c>
+      <c r="C20" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="D20" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="D17" s="23" t="s">
-        <v>25</v>
-      </c>
-      <c r="E17" s="12"/>
-      <c r="F17" s="12"/>
-      <c r="G17" s="12"/>
-    </row>
-    <row r="18" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="3">
-        <v>12</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="E18" s="12"/>
-      <c r="F18" s="12"/>
-      <c r="G18" s="12"/>
-    </row>
-    <row r="19" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="13">
-        <v>13</v>
-      </c>
-      <c r="C19" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="D19" s="23" t="s">
-        <v>25</v>
-      </c>
-      <c r="E19" s="12"/>
-      <c r="F19" s="12"/>
-      <c r="G19" s="12"/>
-    </row>
-    <row r="20" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="10">
-        <v>14</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="D20" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="E20" s="12"/>
-      <c r="F20" s="12"/>
-      <c r="G20" s="12"/>
-    </row>
-    <row r="21" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E20" s="10"/>
+      <c r="F20" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="G20" s="10" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" ht="51" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B21" s="10">
         <v>15</v>
       </c>
-      <c r="C21" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="D21" s="23" t="s">
-        <v>28</v>
-      </c>
-      <c r="E21" s="4"/>
-      <c r="F21" s="4"/>
-      <c r="G21" s="4"/>
-    </row>
-    <row r="22" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C21" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="D21" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="E21" s="23"/>
+      <c r="F21" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="G21" s="10" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B22" s="10">
         <v>16</v>
       </c>
-      <c r="C22" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D22" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E22" s="4"/>
-      <c r="F22" s="4"/>
-      <c r="G22" s="4"/>
-    </row>
-    <row r="23" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C22" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="D22" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="E22" s="10"/>
+      <c r="F22" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="G22" s="10" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B23" s="3">
         <v>17</v>
       </c>
-      <c r="C23" s="4"/>
-      <c r="D23" s="4"/>
-      <c r="E23" s="4"/>
-      <c r="F23" s="4"/>
-      <c r="G23" s="4"/>
-    </row>
-    <row r="24" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="13">
+      <c r="C23" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="D23" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="E23" s="10"/>
+      <c r="F23" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="G23" s="10" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7" ht="47.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B24" s="10">
         <v>18</v>
       </c>
-      <c r="C24" s="4"/>
-      <c r="D24" s="4"/>
-      <c r="E24" s="4"/>
-      <c r="F24" s="4"/>
-      <c r="G24" s="4"/>
-    </row>
-    <row r="25" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C24" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="D24" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="E24" s="10"/>
+      <c r="F24" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="G24" s="10" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B25" s="10">
         <v>19</v>
       </c>
-      <c r="C25" s="4"/>
-      <c r="D25" s="4"/>
+      <c r="C25" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="E25" s="4"/>
-      <c r="F25" s="4"/>
-      <c r="G25" s="4"/>
-    </row>
-    <row r="26" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F25" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="G25" s="4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="26" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B26" s="10">
         <v>20</v>
       </c>
@@ -1523,8 +1701,8 @@
       <c r="F26" s="4"/>
       <c r="G26" s="4"/>
     </row>
-    <row r="27" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="10">
+    <row r="27" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B27" s="3">
         <v>21</v>
       </c>
       <c r="C27" s="4"/>
@@ -1533,8 +1711,8 @@
       <c r="F27" s="4"/>
       <c r="G27" s="4"/>
     </row>
-    <row r="28" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="3">
+    <row r="28" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B28" s="10">
         <v>22</v>
       </c>
       <c r="C28" s="4"/>
@@ -1543,8 +1721,8 @@
       <c r="F28" s="4"/>
       <c r="G28" s="4"/>
     </row>
-    <row r="29" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="13">
+    <row r="29" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B29" s="10">
         <v>23</v>
       </c>
       <c r="C29" s="4"/>
@@ -1553,8 +1731,8 @@
       <c r="F29" s="4"/>
       <c r="G29" s="4"/>
     </row>
-    <row r="30" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="10">
+    <row r="30" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B30" s="3">
         <v>24</v>
       </c>
       <c r="C30" s="4"/>
@@ -1563,7 +1741,7 @@
       <c r="F30" s="4"/>
       <c r="G30" s="4"/>
     </row>
-    <row r="31" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B31" s="10">
         <v>25</v>
       </c>
@@ -1573,7 +1751,7 @@
       <c r="F31" s="4"/>
       <c r="G31" s="4"/>
     </row>
-    <row r="32" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B32" s="10">
         <v>26</v>
       </c>
@@ -1583,7 +1761,7 @@
       <c r="F32" s="4"/>
       <c r="G32" s="4"/>
     </row>
-    <row r="33" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B33" s="3">
         <v>27</v>
       </c>
@@ -1593,8 +1771,8 @@
       <c r="F33" s="4"/>
       <c r="G33" s="4"/>
     </row>
-    <row r="34" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="13">
+    <row r="34" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B34" s="10">
         <v>28</v>
       </c>
       <c r="C34" s="4"/>
@@ -1603,7 +1781,7 @@
       <c r="F34" s="4"/>
       <c r="G34" s="4"/>
     </row>
-    <row r="35" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B35" s="10">
         <v>29</v>
       </c>
@@ -1613,8 +1791,8 @@
       <c r="F35" s="4"/>
       <c r="G35" s="4"/>
     </row>
-    <row r="36" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="10">
+    <row r="36" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B36" s="3">
         <v>30</v>
       </c>
       <c r="C36" s="4"/>
@@ -1623,32 +1801,62 @@
       <c r="F36" s="4"/>
       <c r="G36" s="4"/>
     </row>
-    <row r="37" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B37" s="10">
         <v>31</v>
       </c>
-      <c r="C37" s="5"/>
-      <c r="D37" s="5"/>
-      <c r="E37" s="5"/>
-      <c r="F37" s="5"/>
-      <c r="G37" s="5"/>
-    </row>
-    <row r="39" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B39" s="20" t="s">
+      <c r="C37" s="4"/>
+      <c r="D37" s="4"/>
+      <c r="E37" s="4"/>
+      <c r="F37" s="4"/>
+      <c r="G37" s="4"/>
+    </row>
+    <row r="38" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B38" s="10">
+        <v>32</v>
+      </c>
+      <c r="C38" s="4"/>
+      <c r="D38" s="4"/>
+      <c r="E38" s="4"/>
+      <c r="F38" s="4"/>
+      <c r="G38" s="4"/>
+    </row>
+    <row r="39" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B39" s="3">
+        <v>33</v>
+      </c>
+      <c r="C39" s="4"/>
+      <c r="D39" s="4"/>
+      <c r="E39" s="4"/>
+      <c r="F39" s="4"/>
+      <c r="G39" s="4"/>
+    </row>
+    <row r="40" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B40" s="10">
+        <v>34</v>
+      </c>
+      <c r="C40" s="5"/>
+      <c r="D40" s="5"/>
+      <c r="E40" s="5"/>
+      <c r="F40" s="5"/>
+      <c r="G40" s="5"/>
+    </row>
+    <row r="42" spans="2:7" x14ac:dyDescent="0.45">
+      <c r="B42" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="C39" s="21"/>
-      <c r="D39" s="21"/>
-      <c r="E39" s="21"/>
-      <c r="F39" s="21"/>
-      <c r="G39" s="21"/>
+      <c r="C42" s="22"/>
+      <c r="D42" s="22"/>
+      <c r="E42" s="22"/>
+      <c r="F42" s="22"/>
+      <c r="G42" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="C2:G2"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="C4:D4"/>
-    <mergeCell ref="B39:G39"/>
+    <mergeCell ref="B42:G42"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>

</xml_diff>

<commit_message>
modified the docstring and tests' name
</commit_message>
<xml_diff>
--- a/tests/A01_pixell_test_plan_bank_account.xlsx
+++ b/tests/A01_pixell_test_plan_bank_account.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ADD\Term2\intermediate_software_development\project\Assignment_01\isd_project\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9F9736C-F182-4C9D-AC96-903D6AAE1253}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A208576F-0D09-4EF6-8A5C-FD9642C5113A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6210" yWindow="0" windowWidth="15788" windowHeight="12863" xr2:uid="{8D9DD509-55B1-455D-8036-16809AD15960}"/>
+    <workbookView xWindow="3877" yWindow="683" windowWidth="18241" windowHeight="12480" xr2:uid="{8D9DD509-55B1-455D-8036-16809AD15960}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -183,7 +183,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="57">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -290,51 +290,12 @@
     <t>account_number:"123",       client_number:456,  balance:1000.00</t>
   </si>
   <si>
-    <t>successfully raise ValueError as setted</t>
-  </si>
-  <si>
-    <t>account_number:"123",       client_number:456,  balance:"balance"</t>
-  </si>
-  <si>
-    <t>the value of balance attribute is setted to 0.0 successfully</t>
-  </si>
-  <si>
     <t>account_number:123,       client_number:"456",  balance:1000.00</t>
   </si>
   <si>
-    <t>Balance attribute successfully converted to a float</t>
-  </si>
-  <si>
-    <t>account_number:123,       client_number:"456",  balance:1000</t>
-  </si>
-  <si>
-    <t>the value of balance attribute is converted to a float successfully</t>
-  </si>
-  <si>
-    <t>account_number:123</t>
-  </si>
-  <si>
-    <t>successfully return account_number</t>
-  </si>
-  <si>
-    <t>successfully return client_number</t>
-  </si>
-  <si>
-    <t>client_number:456</t>
-  </si>
-  <si>
-    <t>balance:1000.00</t>
-  </si>
-  <si>
-    <t>successfully return balance</t>
-  </si>
-  <si>
     <t>amount =200</t>
   </si>
   <si>
-    <t>successfully update balance and result is as expected</t>
-  </si>
-  <si>
     <t>amount =-200</t>
   </si>
   <si>
@@ -353,9 +314,6 @@
     <t xml:space="preserve"> raise ValueError  when amount is invalid</t>
   </si>
   <si>
-    <t>successfully added amount to the current balance</t>
-  </si>
-  <si>
     <t>ValueError when amount is non-numeric</t>
   </si>
   <si>
@@ -368,10 +326,34 @@
     <t>amount = 1100</t>
   </si>
   <si>
-    <t>successfully subtract amount from balance</t>
-  </si>
-  <si>
-    <t>successfully return a string as setted</t>
+    <t>None</t>
+  </si>
+  <si>
+    <t>account_number:123,       client_number:456,  balance:"balance"</t>
+  </si>
+  <si>
+    <t>self.bank_account._BankAccount__balance  = 0</t>
+  </si>
+  <si>
+    <t>raises ValueError</t>
+  </si>
+  <si>
+    <t>self.bank_account.account_number = 123</t>
+  </si>
+  <si>
+    <t>self.bank_account.client_number = 456</t>
+  </si>
+  <si>
+    <t>self.bank_account.balance  = 1000.00</t>
+  </si>
+  <si>
+    <t>self.bank_account.balance  = 1200.00</t>
+  </si>
+  <si>
+    <t>self.bank_account.balance  = 800.00</t>
+  </si>
+  <si>
+    <t>"Account Number:123 Balance:$1,000.00"</t>
   </si>
 </sst>
 </file>
@@ -678,7 +660,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
@@ -735,9 +717,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -951,7 +930,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7B0B8C9F-A34D-46F3-9066-19FDAF76B033}" name="Table1" displayName="Table1" ref="B6:G40" totalsRowShown="0" headerRowDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7B0B8C9F-A34D-46F3-9066-19FDAF76B033}" name="Table1" displayName="Table1" ref="B6:G39" totalsRowShown="0" headerRowDxfId="6">
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{B4BB882C-2019-4F87-8900-426FA9A11FFB}" name="Test Case ID" dataDxfId="5"/>
     <tableColumn id="2" xr3:uid="{1904C92F-9639-4229-AA4E-4C4DEAF21EEE}" name="Method being Tested" dataDxfId="4"/>
@@ -1281,20 +1260,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DADEBCC4-BB44-48CD-B9AB-1E2FD3EE0EEB}">
-  <dimension ref="B1:G42"/>
+  <dimension ref="B1:G41"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="2" max="2" width="7.265625" customWidth="1"/>
     <col min="3" max="3" width="16.9296875" customWidth="1"/>
-    <col min="4" max="4" width="30.265625" customWidth="1"/>
-    <col min="5" max="5" width="8.19921875" customWidth="1"/>
-    <col min="6" max="6" width="18.19921875" customWidth="1"/>
-    <col min="7" max="7" width="26.3984375" customWidth="1"/>
+    <col min="4" max="4" width="37.73046875" customWidth="1"/>
+    <col min="5" max="5" width="25.06640625" customWidth="1"/>
+    <col min="6" max="6" width="21.3984375" customWidth="1"/>
+    <col min="7" max="7" width="41.53125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
@@ -1359,7 +1338,9 @@
       <c r="D7" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="E7" s="11"/>
+      <c r="E7" s="11" t="s">
+        <v>47</v>
+      </c>
       <c r="F7" s="11" t="s">
         <v>32</v>
       </c>
@@ -1377,15 +1358,17 @@
       <c r="D8" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E8" s="12"/>
+      <c r="E8" s="12" t="s">
+        <v>47</v>
+      </c>
       <c r="F8" s="11" t="s">
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="G8" s="12" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="9" spans="2:7" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" ht="51.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B9" s="10">
         <v>3</v>
       </c>
@@ -1395,12 +1378,14 @@
       <c r="D9" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="E9" s="12"/>
+      <c r="E9" s="12" t="s">
+        <v>47</v>
+      </c>
       <c r="F9" s="11" t="s">
         <v>34</v>
       </c>
       <c r="G9" s="12" t="s">
-        <v>35</v>
+        <v>50</v>
       </c>
     </row>
     <row r="10" spans="2:7" ht="43.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
@@ -1413,87 +1398,97 @@
       <c r="D10" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="E10" s="12"/>
+      <c r="E10" s="12" t="s">
+        <v>47</v>
+      </c>
       <c r="F10" s="11" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="G10" s="12" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="11" spans="2:7" ht="52.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" ht="42.85" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B11" s="3">
         <v>5</v>
       </c>
-      <c r="C11" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="E11" s="12"/>
+      <c r="C11" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="E11" s="12" t="s">
+        <v>32</v>
+      </c>
       <c r="F11" s="11" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="G11" s="12" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="12" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" ht="42.85" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B12" s="10">
         <v>6</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>14</v>
+        <v>30</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="E12" s="12"/>
-      <c r="F12" s="12" t="s">
-        <v>42</v>
+        <v>31</v>
+      </c>
+      <c r="E12" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="F12" s="11" t="s">
+        <v>47</v>
       </c>
       <c r="G12" s="12" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="13" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" ht="42.85" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B13" s="10">
         <v>7</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="D13" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="E13" s="12"/>
-      <c r="F13" s="12" t="s">
-        <v>45</v>
+        <v>17</v>
+      </c>
+      <c r="E13" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="F13" s="11" t="s">
+        <v>47</v>
       </c>
       <c r="G13" s="12" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="14" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" ht="46.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B14" s="3">
         <v>8</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D14" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="E14" s="10"/>
-      <c r="F14" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="G14" s="10" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="15" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+        <v>19</v>
+      </c>
+      <c r="E14" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="F14" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="G14" s="12" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7" ht="47.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B15" s="10">
         <v>9</v>
       </c>
@@ -1501,17 +1496,19 @@
         <v>18</v>
       </c>
       <c r="D15" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="E15" s="10"/>
-      <c r="F15" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="G15" s="10" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="16" spans="2:7" ht="47.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+        <v>20</v>
+      </c>
+      <c r="E15" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="F15" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="G15" s="12" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B16" s="10">
         <v>10</v>
       </c>
@@ -1519,14 +1516,16 @@
         <v>18</v>
       </c>
       <c r="D16" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="E16" s="10"/>
-      <c r="F16" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="E16" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="F16" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="G16" s="10" t="s">
         <v>50</v>
-      </c>
-      <c r="G16" s="10" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="17" spans="2:7" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
@@ -1534,20 +1533,22 @@
         <v>11</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="D17" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="E17" s="10"/>
-      <c r="F17" s="10" t="s">
-        <v>51</v>
+        <v>42</v>
+      </c>
+      <c r="E17" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="F17" s="11" t="s">
+        <v>38</v>
       </c>
       <c r="G17" s="10" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="18" spans="2:7" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" ht="58.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B18" s="10">
         <v>12</v>
       </c>
@@ -1555,17 +1556,19 @@
         <v>23</v>
       </c>
       <c r="D18" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="E18" s="10"/>
-      <c r="F18" s="10" t="s">
-        <v>51</v>
+        <v>25</v>
+      </c>
+      <c r="E18" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="F18" s="11" t="s">
+        <v>40</v>
       </c>
       <c r="G18" s="10" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="19" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" ht="51" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B19" s="10">
         <v>13</v>
       </c>
@@ -1573,35 +1576,39 @@
         <v>23</v>
       </c>
       <c r="D19" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="E19" s="10"/>
-      <c r="F19" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="G19" s="10" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="20" spans="2:7" ht="51" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+        <v>24</v>
+      </c>
+      <c r="E19" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="F19" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="G19" s="12" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" ht="46.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B20" s="3">
         <v>14</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D20" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="E20" s="10"/>
-      <c r="F20" s="10" t="s">
-        <v>52</v>
+        <v>43</v>
+      </c>
+      <c r="E20" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="F20" s="11" t="s">
+        <v>38</v>
       </c>
       <c r="G20" s="10" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="21" spans="2:7" ht="51" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" ht="42.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B21" s="10">
         <v>15</v>
       </c>
@@ -1609,17 +1616,19 @@
         <v>26</v>
       </c>
       <c r="D21" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="E21" s="23"/>
+        <v>44</v>
+      </c>
+      <c r="E21" s="12" t="s">
+        <v>32</v>
+      </c>
       <c r="F21" s="10" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="G21" s="10" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="22" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" ht="46.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B22" s="10">
         <v>16</v>
       </c>
@@ -1627,17 +1636,19 @@
         <v>26</v>
       </c>
       <c r="D22" s="10" t="s">
-        <v>58</v>
-      </c>
-      <c r="E22" s="10"/>
+        <v>27</v>
+      </c>
+      <c r="E22" s="12" t="s">
+        <v>32</v>
+      </c>
       <c r="F22" s="10" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
       <c r="G22" s="10" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="23" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7" ht="47.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B23" s="3">
         <v>17</v>
       </c>
@@ -1645,54 +1656,50 @@
         <v>26</v>
       </c>
       <c r="D23" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="E23" s="10"/>
+        <v>24</v>
+      </c>
+      <c r="E23" s="12" t="s">
+        <v>32</v>
+      </c>
       <c r="F23" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="G23" s="10" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="24" spans="2:7" ht="47.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+        <v>36</v>
+      </c>
+      <c r="G23" s="12" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B24" s="10">
         <v>18</v>
       </c>
-      <c r="C24" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="D24" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="E24" s="10"/>
-      <c r="F24" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="G24" s="10" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="25" spans="2:7" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="C24" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E24" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="F24" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="G24" s="4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B25" s="10">
         <v>19</v>
       </c>
-      <c r="C25" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D25" s="4" t="s">
-        <v>22</v>
-      </c>
+      <c r="C25" s="4"/>
+      <c r="D25" s="4"/>
       <c r="E25" s="4"/>
-      <c r="F25" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="G25" s="4" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="26" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B26" s="10">
+      <c r="F25" s="4"/>
+      <c r="G25" s="4"/>
+    </row>
+    <row r="26" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B26" s="3">
         <v>20</v>
       </c>
       <c r="C26" s="4"/>
@@ -1702,7 +1709,7 @@
       <c r="G26" s="4"/>
     </row>
     <row r="27" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B27" s="3">
+      <c r="B27" s="10">
         <v>21</v>
       </c>
       <c r="C27" s="4"/>
@@ -1711,7 +1718,7 @@
       <c r="F27" s="4"/>
       <c r="G27" s="4"/>
     </row>
-    <row r="28" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="28" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B28" s="10">
         <v>22</v>
       </c>
@@ -1721,8 +1728,8 @@
       <c r="F28" s="4"/>
       <c r="G28" s="4"/>
     </row>
-    <row r="29" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B29" s="10">
+    <row r="29" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B29" s="3">
         <v>23</v>
       </c>
       <c r="C29" s="4"/>
@@ -1732,7 +1739,7 @@
       <c r="G29" s="4"/>
     </row>
     <row r="30" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B30" s="3">
+      <c r="B30" s="10">
         <v>24</v>
       </c>
       <c r="C30" s="4"/>
@@ -1741,7 +1748,7 @@
       <c r="F30" s="4"/>
       <c r="G30" s="4"/>
     </row>
-    <row r="31" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="31" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B31" s="10">
         <v>25</v>
       </c>
@@ -1751,8 +1758,8 @@
       <c r="F31" s="4"/>
       <c r="G31" s="4"/>
     </row>
-    <row r="32" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B32" s="10">
+    <row r="32" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B32" s="3">
         <v>26</v>
       </c>
       <c r="C32" s="4"/>
@@ -1762,7 +1769,7 @@
       <c r="G32" s="4"/>
     </row>
     <row r="33" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B33" s="3">
+      <c r="B33" s="10">
         <v>27</v>
       </c>
       <c r="C33" s="4"/>
@@ -1771,7 +1778,7 @@
       <c r="F33" s="4"/>
       <c r="G33" s="4"/>
     </row>
-    <row r="34" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="34" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B34" s="10">
         <v>28</v>
       </c>
@@ -1781,8 +1788,8 @@
       <c r="F34" s="4"/>
       <c r="G34" s="4"/>
     </row>
-    <row r="35" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B35" s="10">
+    <row r="35" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B35" s="3">
         <v>29</v>
       </c>
       <c r="C35" s="4"/>
@@ -1792,7 +1799,7 @@
       <c r="G35" s="4"/>
     </row>
     <row r="36" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B36" s="3">
+      <c r="B36" s="10">
         <v>30</v>
       </c>
       <c r="C36" s="4"/>
@@ -1801,7 +1808,7 @@
       <c r="F36" s="4"/>
       <c r="G36" s="4"/>
     </row>
-    <row r="37" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="37" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B37" s="10">
         <v>31</v>
       </c>
@@ -1811,8 +1818,8 @@
       <c r="F37" s="4"/>
       <c r="G37" s="4"/>
     </row>
-    <row r="38" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B38" s="10">
+    <row r="38" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B38" s="3">
         <v>32</v>
       </c>
       <c r="C38" s="4"/>
@@ -1822,41 +1829,31 @@
       <c r="G38" s="4"/>
     </row>
     <row r="39" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B39" s="3">
+      <c r="B39" s="10">
         <v>33</v>
       </c>
-      <c r="C39" s="4"/>
-      <c r="D39" s="4"/>
-      <c r="E39" s="4"/>
-      <c r="F39" s="4"/>
-      <c r="G39" s="4"/>
-    </row>
-    <row r="40" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B40" s="10">
-        <v>34</v>
-      </c>
-      <c r="C40" s="5"/>
-      <c r="D40" s="5"/>
-      <c r="E40" s="5"/>
-      <c r="F40" s="5"/>
-      <c r="G40" s="5"/>
-    </row>
-    <row r="42" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="B42" s="21" t="s">
+      <c r="C39" s="5"/>
+      <c r="D39" s="5"/>
+      <c r="E39" s="5"/>
+      <c r="F39" s="5"/>
+      <c r="G39" s="5"/>
+    </row>
+    <row r="41" spans="2:7" x14ac:dyDescent="0.45">
+      <c r="B41" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="C42" s="22"/>
-      <c r="D42" s="22"/>
-      <c r="E42" s="22"/>
-      <c r="F42" s="22"/>
-      <c r="G42" s="22"/>
+      <c r="C41" s="22"/>
+      <c r="D41" s="22"/>
+      <c r="E41" s="22"/>
+      <c r="F41" s="22"/>
+      <c r="G41" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="C2:G2"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="C4:D4"/>
-    <mergeCell ref="B42:G42"/>
+    <mergeCell ref="B41:G41"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>

</xml_diff>

<commit_message>
completed bank_account.py and chequing_account.py and the tests
</commit_message>
<xml_diff>
--- a/tests/A01_pixell_test_plan_bank_account.xlsx
+++ b/tests/A01_pixell_test_plan_bank_account.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ADD\Term2\intermediate_software_development\project\Assignment_01\isd_project\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A208576F-0D09-4EF6-8A5C-FD9642C5113A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F320C64E-A3B2-44A6-A336-61298D846690}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3877" yWindow="683" windowWidth="18241" windowHeight="12480" xr2:uid="{8D9DD509-55B1-455D-8036-16809AD15960}"/>
+    <workbookView xWindow="1013" yWindow="1020" windowWidth="20587" windowHeight="12480" xr2:uid="{8D9DD509-55B1-455D-8036-16809AD15960}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1263,7 +1263,7 @@
   <dimension ref="B1:G41"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>

<commit_message>
completed the investment account file and the tests
</commit_message>
<xml_diff>
--- a/tests/A01_pixell_test_plan_bank_account.xlsx
+++ b/tests/A01_pixell_test_plan_bank_account.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ADD\Term2\intermediate_software_development\project\Assignment_01\isd_project\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F320C64E-A3B2-44A6-A336-61298D846690}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93FBFC74-2505-48F9-8DF8-E66ACB5ADF3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1013" yWindow="1020" windowWidth="20587" windowHeight="12480" xr2:uid="{8D9DD509-55B1-455D-8036-16809AD15960}"/>
+    <workbookView xWindow="2573" yWindow="1020" windowWidth="18397" windowHeight="12480" xr2:uid="{8D9DD509-55B1-455D-8036-16809AD15960}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>

</xml_diff>